<commit_message>
Feat: Implement new logic for unexpected replicate handling
- Introduces new logic for handling unexpected replicates when one is
  contaminated.
- A new column, unexpected_replicate_status, is added to subject_qc.csv
  to reflect the updated handling.
- Additionally, the description for the unexpected_replicate_status
  column has been updated in QC_Report_Data_Dictionary.xlsx
</commit_message>
<xml_diff>
--- a/src/cgr_gwas_qc/reporting/QC_Report_Data_Dictionary.xlsx
+++ b/src/cgr_gwas_qc/reporting/QC_Report_Data_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://researchtriangleinstitute-my.sharepoint.com/personal/jmarks_rti_org/Documents/Projects/nci_cgr/dev-tests/019/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\DCEG\Home\marksja\github\GwasQcPipeline\src\cgr_gwas_qc\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="8_{2F0C6400-AD89-0F4B-8A91-6CFC3B64BB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8FC98F3-2A55-DB42-A941-A4425994AD7A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59492EAE-3006-47B3-8F45-BE8862A898A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{EC8BB56D-BE63-6F4D-9B7A-02D3F7D32CB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27120" windowHeight="16440" activeTab="2" xr2:uid="{EC8BB56D-BE63-6F4D-9B7A-02D3F7D32CB1}"/>
   </bookViews>
   <sheets>
     <sheet name="SAMPLE_QC_DD" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="150">
   <si>
     <t>ADDITIONAL COLUMNS</t>
   </si>
@@ -175,7 +175,7 @@
   </si>
   <si>
     <r>
-      <t>1=</t>
+      <t>0=</t>
     </r>
     <r>
       <rPr>
@@ -193,12 +193,695 @@
         <rFont val="Helvetica"/>
         <family val="2"/>
       </rPr>
-      <t>: unexpected replicate (only the other sample is contaminated)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>0=</t>
+      <t>: not an unexpected replicate</t>
+    </r>
+  </si>
+  <si>
+    <t>Identifies unexpected replicates and their retainment status after contamination assessment.</t>
+  </si>
+  <si>
+    <t>unexpected_replicate_status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown=Unknown Case/Control status </t>
+  </si>
+  <si>
+    <t>QC=Quality Control</t>
+  </si>
+  <si>
+    <t>Control=Control</t>
+  </si>
+  <si>
+    <t>Case=Case</t>
+  </si>
+  <si>
+    <t>CASE_CONTROL_DTYPE</t>
+  </si>
+  <si>
+    <t>Case/Control_Status</t>
+  </si>
+  <si>
+    <t>The sample identifier used by the workflow.</t>
+  </si>
+  <si>
+    <t>Sample_ID</t>
+  </si>
+  <si>
+    <t>Group_By_Subject_ID</t>
+  </si>
+  <si>
+    <t>VALUES</t>
+  </si>
+  <si>
+    <t>DTYPE</t>
+  </si>
+  <si>
+    <t>VARDESC</t>
+  </si>
+  <si>
+    <t>VARNAME</t>
+  </si>
+  <si>
+    <t>Phenotype status.</t>
+  </si>
+  <si>
+    <t>The subject identifier used by the workflow.</t>
+  </si>
+  <si>
+    <t>These columns and their associated values were extracted from the cgr_sample_sheet.csv.</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Internal Control</t>
+  </si>
+  <si>
+    <t>Number Samples Per Subject</t>
+  </si>
+  <si>
+    <t>Replicate IDs</t>
+  </si>
+  <si>
+    <t>Sample Excluded from QC</t>
+  </si>
+  <si>
+    <t>Sample Used in Subject Analysis</t>
+  </si>
+  <si>
+    <t>Subject Removed</t>
+  </si>
+  <si>
+    <t>Sample Pass QC</t>
+  </si>
+  <si>
+    <t>Low Call Rate</t>
+  </si>
+  <si>
+    <t>Call_Rate_Initial</t>
+  </si>
+  <si>
+    <t>Call_Rate_1_filter</t>
+  </si>
+  <si>
+    <t>Call_Rate_1</t>
+  </si>
+  <si>
+    <t>Call_Rate_2_filter</t>
+  </si>
+  <si>
+    <t>Call_Rate_2</t>
+  </si>
+  <si>
+    <t>Contaminated</t>
+  </si>
+  <si>
+    <t>Contamination_Rate</t>
+  </si>
+  <si>
+    <t>IdatIntensity</t>
+  </si>
+  <si>
+    <t>Expected Replicate Discordance</t>
+  </si>
+  <si>
+    <t>Count_of_QC_Issue</t>
+  </si>
+  <si>
+    <t>Extracted from cgr_sample_qc.csv</t>
+  </si>
+  <si>
+    <t>UInt32</t>
+  </si>
+  <si>
+    <t>The total number of Sample_ID per Group_By_Subject_ID</t>
+  </si>
+  <si>
+    <t>Concatenated Sample_IDs that are replicates.</t>
+  </si>
+  <si>
+    <t>True if the sample failed QC criteria.</t>
+  </si>
+  <si>
+    <t>True if the Sample_ID is used to represent the subject.</t>
+  </si>
+  <si>
+    <t>True if there are no samples passing QC for this subject.</t>
+  </si>
+  <si>
+    <t>True if the sample passed all QC metrics:     "is_call_rate_filtered", "is_contaminated", "Expected Replicate Discordance", "Unexpected Replicate", and "is_sex_discordant"</t>
+  </si>
+  <si>
+    <t>True if a sample was removed by either call rate filter.</t>
+  </si>
+  <si>
+    <t>The Initial sample call rate before any filters.</t>
+  </si>
+  <si>
+    <t>The sample call rate after the first filter.</t>
+  </si>
+  <si>
+    <t>True if a sample was removed by the first call rate filter.</t>
+  </si>
+  <si>
+    <t>True if a sample was removed by the second call rate filter.</t>
+  </si>
+  <si>
+    <t>The sample call rate after the second filter.</t>
+  </si>
+  <si>
+    <t>True if a sample exceed the contamination rate threshold.</t>
+  </si>
+  <si>
+    <t>The SNPweights contamination rate (%Mix)</t>
+  </si>
+  <si>
+    <t>The median IDAT intensity.</t>
+  </si>
+  <si>
+    <t>True if the replicates had low concordance.</t>
+  </si>
+  <si>
+    <t>Number of issues encountered when examining the following QC metrics: 'is_call_rate_filtered,' 'is_contaminated,' 'Expected Replicate Discordance,' 'Unexpected Replicate,' and 'is_sex_discordant.'</t>
+  </si>
+  <si>
+    <t>Sample_ID1</t>
+  </si>
+  <si>
+    <t>Sample_ID2</t>
+  </si>
+  <si>
+    <t>Subject_ID1</t>
+  </si>
+  <si>
+    <t>Subject_ID2</t>
+  </si>
+  <si>
+    <t>Case/Control_Status1</t>
+  </si>
+  <si>
+    <t>Case/Control_Status2</t>
+  </si>
+  <si>
+    <t>Sample Used in Subject Analysis1</t>
+  </si>
+  <si>
+    <t>Sample Used in Subject Analysis2</t>
+  </si>
+  <si>
+    <t>Ancestry1</t>
+  </si>
+  <si>
+    <t>Ancestry2</t>
+  </si>
+  <si>
+    <t>Expected Replicate</t>
+  </si>
+  <si>
+    <t>PLINK_PI_HAT</t>
+  </si>
+  <si>
+    <t>PLINK_concordance</t>
+  </si>
+  <si>
+    <t>PLINK_is_ge_pi_hat</t>
+  </si>
+  <si>
+    <t>PLINK_is_ge_concordance</t>
+  </si>
+  <si>
+    <t>GRAF_HGMR</t>
+  </si>
+  <si>
+    <t>GRAF_AGMR</t>
+  </si>
+  <si>
+    <t>GRAF_relationship</t>
+  </si>
+  <si>
+    <t>KING_Kinship</t>
+  </si>
+  <si>
+    <t>KING_relationship</t>
+  </si>
+  <si>
+    <t>Sample_ID for the first sample in the pairwise comparison.</t>
+  </si>
+  <si>
+    <t>Sample_ID for the second sample in the pairwise comparison.</t>
+  </si>
+  <si>
+    <t>Subject_ID for the first sample in the pairwise comparison.</t>
+  </si>
+  <si>
+    <t>Subject_ID for the second sample in the pairwise comparison.</t>
+  </si>
+  <si>
+    <t>Case/Control information for the first sample in the pairwise comparison.</t>
+  </si>
+  <si>
+    <t>Case/Control information for the second sample in the pairwise comparison.</t>
+  </si>
+  <si>
+    <t>True if the pair of samples are known replicates.</t>
+  </si>
+  <si>
+    <t>Proportion IBD i.e. ``P(IBD=2) + 0.5 * P(IBD=1)``</t>
+  </si>
+  <si>
+    <t>Proportion IBS2 ``IBS2 / (IBS0 + IBS1 + IBS2)``</t>
+  </si>
+  <si>
+    <t>True if PI_HAT was greater than ``software_params.pi_hat_cutoff``</t>
+  </si>
+  <si>
+    <t>The assigned relationship based on Kinship</t>
+  </si>
+  <si>
+    <t>Estimated kinship coefficient from the SNP data</t>
+  </si>
+  <si>
+    <t>Relationship determined by sample genotypes.</t>
+  </si>
+  <si>
+    <t>All Genotype Mismatch Rate (%)</t>
+  </si>
+  <si>
+    <t>Homozygous Genotype Mismatch Rate (%)</t>
+  </si>
+  <si>
+    <t>Assigned ancestral population (GRAF) of Sample_ID1.</t>
+  </si>
+  <si>
+    <t>Assigned ancestral population (GRAF) of Sample_ID2.</t>
+  </si>
+  <si>
+    <t>True if Sample_ID1 used in Subject Analysis</t>
+  </si>
+  <si>
+    <t>True if Sample_ID2 used in Subject Analysis</t>
+  </si>
+  <si>
+    <t>#SNPs</t>
+  </si>
+  <si>
+    <t>GD1 (x)</t>
+  </si>
+  <si>
+    <t>GD2 (y)</t>
+  </si>
+  <si>
+    <t>GD3 (z)</t>
+  </si>
+  <si>
+    <t>GD4</t>
+  </si>
+  <si>
+    <t>F(%)</t>
+  </si>
+  <si>
+    <t>E(%)</t>
+  </si>
+  <si>
+    <t>A(%)</t>
+  </si>
+  <si>
+    <t>This table outlines the key variables and their descriptions from the Subject QC workflow/analyses. </t>
+  </si>
+  <si>
+    <t>The Concordance Checks table provides detailed information about pairwise comparisons of samples to assess their genetic similarity and relatedness.</t>
+  </si>
+  <si>
+    <t>The SAMPLE QC table outlines the key variables and their descriptions from the Sample QC workflow/analyses. </t>
+  </si>
+  <si>
+    <t>The proportion of African ancestry in the sample.</t>
+  </si>
+  <si>
+    <t>The proportion of European ancestry in the sample.</t>
+  </si>
+  <si>
+    <t>The proportion of Asian ancestry in the sample.</t>
+  </si>
+  <si>
+    <t>Inferring subject ancestry with genotypes using Grafpop: https://www.ncbi.nlm.nih.gov/projects/gap/cgi-bin/GrafPop_README.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Calculate the genetic distances </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from subject </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the last two reference populations South Asian and Mexican/Latino. The difference </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, called GD4 score</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> coordinate of point </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> after transformation (step 7), called GD3 score, is also used for plotting results.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Plot the converted Cartesian coordinates of subject </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, together with ΔEFA</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, on the </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x-y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> plane. The final </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i0</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> values are the normalized genetic distances, called GD1 and GD2 scores</t>
+    </r>
+  </si>
+  <si>
+    <t>Number of SNPs used to calculate the subsequent distance metrics (GD1, GD2, GD3, GD4) and ancestry proportions (E%, F%, A%).</t>
+  </si>
+  <si>
+    <t>Uint32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>UNEXPECTED_REPLICATE_STATUS_DTYPE</t>
+  </si>
+  <si>
+    <r>
+      <t>1=</t>
     </r>
     <r>
       <rPr>
@@ -216,688 +899,8 @@
         <rFont val="Helvetica"/>
         <family val="2"/>
       </rPr>
-      <t>: not an unexpected replicate</t>
-    </r>
-  </si>
-  <si>
-    <t>Identifies unexpected replicates and their retainment status after contamination assessment.</t>
-  </si>
-  <si>
-    <t>unexpected_replicate_status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown=Unknown Case/Control status </t>
-  </si>
-  <si>
-    <t>QC=Quality Control</t>
-  </si>
-  <si>
-    <t>Control=Control</t>
-  </si>
-  <si>
-    <t>Case=Case</t>
-  </si>
-  <si>
-    <t>CASE_CONTROL_DTYPE</t>
-  </si>
-  <si>
-    <t>Case/Control_Status</t>
-  </si>
-  <si>
-    <t>The sample identifier used by the workflow.</t>
-  </si>
-  <si>
-    <t>Sample_ID</t>
-  </si>
-  <si>
-    <t>Group_By_Subject_ID</t>
-  </si>
-  <si>
-    <t>VALUES</t>
-  </si>
-  <si>
-    <t>DTYPE</t>
-  </si>
-  <si>
-    <t>VARDESC</t>
-  </si>
-  <si>
-    <t>VARNAME</t>
-  </si>
-  <si>
-    <t>Phenotype status.</t>
-  </si>
-  <si>
-    <t>The subject identifier used by the workflow.</t>
-  </si>
-  <si>
-    <t>These columns and their associated values were extracted from the cgr_sample_sheet.csv.</t>
-  </si>
-  <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Internal Control</t>
-  </si>
-  <si>
-    <t>Number Samples Per Subject</t>
-  </si>
-  <si>
-    <t>Replicate IDs</t>
-  </si>
-  <si>
-    <t>Sample Excluded from QC</t>
-  </si>
-  <si>
-    <t>Sample Used in Subject Analysis</t>
-  </si>
-  <si>
-    <t>Subject Removed</t>
-  </si>
-  <si>
-    <t>Sample Pass QC</t>
-  </si>
-  <si>
-    <t>Low Call Rate</t>
-  </si>
-  <si>
-    <t>Call_Rate_Initial</t>
-  </si>
-  <si>
-    <t>Call_Rate_1_filter</t>
-  </si>
-  <si>
-    <t>Call_Rate_1</t>
-  </si>
-  <si>
-    <t>Call_Rate_2_filter</t>
-  </si>
-  <si>
-    <t>Call_Rate_2</t>
-  </si>
-  <si>
-    <t>Contaminated</t>
-  </si>
-  <si>
-    <t>Contamination_Rate</t>
-  </si>
-  <si>
-    <t>IdatIntensity</t>
-  </si>
-  <si>
-    <t>Expected Replicate Discordance</t>
-  </si>
-  <si>
-    <t>Count_of_QC_Issue</t>
-  </si>
-  <si>
-    <t>Extracted from cgr_sample_qc.csv</t>
-  </si>
-  <si>
-    <t>UInt32</t>
-  </si>
-  <si>
-    <t>The total number of Sample_ID per Group_By_Subject_ID</t>
-  </si>
-  <si>
-    <t>Concatenated Sample_IDs that are replicates.</t>
-  </si>
-  <si>
-    <t>True if the sample failed QC criteria.</t>
-  </si>
-  <si>
-    <t>True if the Sample_ID is used to represent the subject.</t>
-  </si>
-  <si>
-    <t>True if there are no samples passing QC for this subject.</t>
-  </si>
-  <si>
-    <t>True if the sample passed all QC metrics:     "is_call_rate_filtered", "is_contaminated", "Expected Replicate Discordance", "Unexpected Replicate", and "is_sex_discordant"</t>
-  </si>
-  <si>
-    <t>True if a sample was removed by either call rate filter.</t>
-  </si>
-  <si>
-    <t>The Initial sample call rate before any filters.</t>
-  </si>
-  <si>
-    <t>The sample call rate after the first filter.</t>
-  </si>
-  <si>
-    <t>True if a sample was removed by the first call rate filter.</t>
-  </si>
-  <si>
-    <t>True if a sample was removed by the second call rate filter.</t>
-  </si>
-  <si>
-    <t>The sample call rate after the second filter.</t>
-  </si>
-  <si>
-    <t>True if a sample exceed the contamination rate threshold.</t>
-  </si>
-  <si>
-    <t>The SNPweights contamination rate (%Mix)</t>
-  </si>
-  <si>
-    <t>The median IDAT intensity.</t>
-  </si>
-  <si>
-    <t>True if the replicates had low concordance.</t>
-  </si>
-  <si>
-    <t>Number of issues encountered when examining the following QC metrics: 'is_call_rate_filtered,' 'is_contaminated,' 'Expected Replicate Discordance,' 'Unexpected Replicate,' and 'is_sex_discordant.'</t>
-  </si>
-  <si>
-    <t>Sample_ID1</t>
-  </si>
-  <si>
-    <t>Sample_ID2</t>
-  </si>
-  <si>
-    <t>Subject_ID1</t>
-  </si>
-  <si>
-    <t>Subject_ID2</t>
-  </si>
-  <si>
-    <t>Case/Control_Status1</t>
-  </si>
-  <si>
-    <t>Case/Control_Status2</t>
-  </si>
-  <si>
-    <t>Sample Used in Subject Analysis1</t>
-  </si>
-  <si>
-    <t>Sample Used in Subject Analysis2</t>
-  </si>
-  <si>
-    <t>Ancestry1</t>
-  </si>
-  <si>
-    <t>Ancestry2</t>
-  </si>
-  <si>
-    <t>Expected Replicate</t>
-  </si>
-  <si>
-    <t>PLINK_PI_HAT</t>
-  </si>
-  <si>
-    <t>PLINK_concordance</t>
-  </si>
-  <si>
-    <t>PLINK_is_ge_pi_hat</t>
-  </si>
-  <si>
-    <t>PLINK_is_ge_concordance</t>
-  </si>
-  <si>
-    <t>GRAF_HGMR</t>
-  </si>
-  <si>
-    <t>GRAF_AGMR</t>
-  </si>
-  <si>
-    <t>GRAF_relationship</t>
-  </si>
-  <si>
-    <t>KING_Kinship</t>
-  </si>
-  <si>
-    <t>KING_relationship</t>
-  </si>
-  <si>
-    <t>Sample_ID for the first sample in the pairwise comparison.</t>
-  </si>
-  <si>
-    <t>Sample_ID for the second sample in the pairwise comparison.</t>
-  </si>
-  <si>
-    <t>Subject_ID for the first sample in the pairwise comparison.</t>
-  </si>
-  <si>
-    <t>Subject_ID for the second sample in the pairwise comparison.</t>
-  </si>
-  <si>
-    <t>Case/Control information for the first sample in the pairwise comparison.</t>
-  </si>
-  <si>
-    <t>Case/Control information for the second sample in the pairwise comparison.</t>
-  </si>
-  <si>
-    <t>True if the pair of samples are known replicates.</t>
-  </si>
-  <si>
-    <t>Proportion IBD i.e. ``P(IBD=2) + 0.5 * P(IBD=1)``</t>
-  </si>
-  <si>
-    <t>Proportion IBS2 ``IBS2 / (IBS0 + IBS1 + IBS2)``</t>
-  </si>
-  <si>
-    <t>True if PI_HAT was greater than ``software_params.pi_hat_cutoff``</t>
-  </si>
-  <si>
-    <t>The assigned relationship based on Kinship</t>
-  </si>
-  <si>
-    <t>Estimated kinship coefficient from the SNP data</t>
-  </si>
-  <si>
-    <t>Relationship determined by sample genotypes.</t>
-  </si>
-  <si>
-    <t>All Genotype Mismatch Rate (%)</t>
-  </si>
-  <si>
-    <t>Homozygous Genotype Mismatch Rate (%)</t>
-  </si>
-  <si>
-    <t>Assigned ancestral population (GRAF) of Sample_ID1.</t>
-  </si>
-  <si>
-    <t>Assigned ancestral population (GRAF) of Sample_ID2.</t>
-  </si>
-  <si>
-    <t>True if Sample_ID1 used in Subject Analysis</t>
-  </si>
-  <si>
-    <t>True if Sample_ID2 used in Subject Analysis</t>
-  </si>
-  <si>
-    <t>#SNPs</t>
-  </si>
-  <si>
-    <t>GD1 (x)</t>
-  </si>
-  <si>
-    <t>GD2 (y)</t>
-  </si>
-  <si>
-    <t>GD3 (z)</t>
-  </si>
-  <si>
-    <t>GD4</t>
-  </si>
-  <si>
-    <t>F(%)</t>
-  </si>
-  <si>
-    <t>E(%)</t>
-  </si>
-  <si>
-    <t>A(%)</t>
-  </si>
-  <si>
-    <t>This table outlines the key variables and their descriptions from the Subject QC workflow/analyses. </t>
-  </si>
-  <si>
-    <t>The Concordance Checks table provides detailed information about pairwise comparisons of samples to assess their genetic similarity and relatedness.</t>
-  </si>
-  <si>
-    <t>The SAMPLE QC table outlines the key variables and their descriptions from the Sample QC workflow/analyses. </t>
-  </si>
-  <si>
-    <t>The proportion of African ancestry in the sample.</t>
-  </si>
-  <si>
-    <t>The proportion of European ancestry in the sample.</t>
-  </si>
-  <si>
-    <t>The proportion of Asian ancestry in the sample.</t>
-  </si>
-  <si>
-    <t>Inferring subject ancestry with genotypes using Grafpop: https://www.ncbi.nlm.nih.gov/projects/gap/cgi-bin/GrafPop_README.html</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Calculate the genetic distances </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> from subject </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to the last two reference populations South Asian and Mexican/Latino. The difference </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> - </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, called GD4 score</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>z</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> coordinate of point </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Q</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> after transformation (step 7), called GD3 score, is also used for plotting results.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Plot the converted Cartesian coordinates of subject </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, together with ΔEFA</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, on the </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x-y</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> plane. The final </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i0</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>y</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> values are the normalized genetic distances, called GD1 and GD2 scores</t>
-    </r>
-  </si>
-  <si>
-    <t>Number of SNPs used to calculate the subsequent distance metrics (GD1, GD2, GD3, GD4) and ancestry proportions (E%, F%, A%).</t>
-  </si>
-  <si>
-    <t>Uint32</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+      <t>: unexpected replicate (contamination only present in the other sample)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1426,99 +1429,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44C1C36-A81F-1341-8CED-1D622F1C199A}">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A6" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1530,34 +1533,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>72</v>
-      </c>
-      <c r="C10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>73</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -1569,12 +1572,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1583,12 +1586,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1600,12 +1603,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -1617,12 +1620,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -1634,23 +1637,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1662,23 +1665,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1690,23 +1693,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -1718,34 +1721,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1757,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -1774,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1791,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1853,7 +1856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1864,7 +1867,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -1886,98 +1889,98 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
     </row>
   </sheetData>
@@ -1996,103 +1999,103 @@
       <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -2101,12 +2104,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -2115,34 +2118,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
@@ -2154,12 +2157,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -2171,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -2188,34 +2191,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -2227,12 +2230,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -2244,167 +2247,167 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
     </row>
   </sheetData>
@@ -2419,180 +2422,180 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00489465-F65E-564F-9966-7808F489929B}">
   <dimension ref="A1:AV58"/>
   <sheetViews>
-    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:G4"/>
+    <sheetView tabSelected="1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="E10" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
-      <c r="AM9" s="1"/>
-      <c r="AN9" s="1"/>
-      <c r="AO9" s="1"/>
-      <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
-      <c r="AR9" s="1"/>
-      <c r="AS9" s="1"/>
-      <c r="AT9" s="1"/>
-      <c r="AU9" s="1"/>
-      <c r="AV9" s="1"/>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2632,7 +2635,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -2644,7 +2647,7 @@
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2661,7 +2664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2672,7 +2675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2683,7 +2686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -2694,7 +2697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2705,114 +2708,114 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
     </row>
   </sheetData>
@@ -2831,60 +2834,60 @@
       <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -2893,106 +2896,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>

</xml_diff>